<commit_message>
Some mods to Altium Design
</commit_message>
<xml_diff>
--- a/CHIPS Documents/CHIPS Budget.xlsx
+++ b/CHIPS Documents/CHIPS Budget.xlsx
@@ -171,9 +171,6 @@
     <t>Coax Connector</t>
   </si>
   <si>
-    <t>DSPIC33EP510MG310-I/PT-ND</t>
-  </si>
-  <si>
     <t>Programming Header</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   </si>
   <si>
     <t>TFML-125-02-L-D</t>
+  </si>
+  <si>
+    <t>DSPIC33EP510MU810-I/PT-ND</t>
   </si>
 </sst>
 </file>
@@ -840,7 +840,7 @@
   <dimension ref="B1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2">
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
@@ -1263,7 +1263,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>37</v>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1330,7 +1330,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>38</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E29" s="13">
         <v>5</v>
@@ -1365,18 +1365,18 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="E30" s="2">
         <v>8</v>
@@ -1387,7 +1387,7 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
@@ -1395,10 +1395,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
@@ -1416,10 +1416,10 @@
         <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
@@ -1432,7 +1432,7 @@
         <v>49.95</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
@@ -1487,7 +1487,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>38</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>38</v>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>

</xml_diff>

<commit_message>
Initial Altium Rev for uC
</commit_message>
<xml_diff>
--- a/CHIPS Documents/CHIPS Budget.xlsx
+++ b/CHIPS Documents/CHIPS Budget.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="69">
   <si>
     <t>Item</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Microcontroller</t>
   </si>
   <si>
-    <t>FTDI Cable</t>
-  </si>
-  <si>
     <t>Programmer</t>
   </si>
   <si>
@@ -207,28 +204,28 @@
     <t>SFML-125-02-L-DH</t>
   </si>
   <si>
-    <t>10 MHz Crystal</t>
-  </si>
-  <si>
-    <t>535-9065-1-ND</t>
-  </si>
-  <si>
-    <t>CKN4080-ND</t>
-  </si>
-  <si>
     <t>Sample, have extras</t>
   </si>
   <si>
-    <t>DEV-09717</t>
-  </si>
-  <si>
     <t>TSW-106-07-F-S</t>
   </si>
   <si>
     <t>TFML-125-02-L-D</t>
   </si>
   <si>
-    <t>DSPIC33EP510MU810-I/PT-ND</t>
+    <t>Borrow from Trudy</t>
+  </si>
+  <si>
+    <t>300-6145-1-ND</t>
+  </si>
+  <si>
+    <t>24 MHz Crystal</t>
+  </si>
+  <si>
+    <t>732-7013-1-ND</t>
+  </si>
+  <si>
+    <t>PIC32MZ2048EFH144-I/PL-ND</t>
   </si>
 </sst>
 </file>
@@ -837,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L53"/>
+  <dimension ref="B1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>4</v>
@@ -899,10 +896,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="13">
         <v>1</v>
@@ -918,8 +915,8 @@
         <v>4</v>
       </c>
       <c r="K4" s="5">
-        <f>SUM(G4:G11,G15:G24,G28:G37,G41:G52)</f>
-        <v>1839.45</v>
+        <f>SUM(G4:G11,G15:G24,G28:G36,G40:G51)</f>
+        <v>1826.95</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -927,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
@@ -948,10 +945,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -969,10 +966,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2">
         <v>4</v>
@@ -985,7 +982,7 @@
         <v>800</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
@@ -993,10 +990,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2">
         <v>1</v>
@@ -1015,10 +1012,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2">
         <v>3</v>
@@ -1037,10 +1034,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
@@ -1059,10 +1056,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2">
         <v>4</v>
@@ -1081,7 +1078,7 @@
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
       <c r="F12" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="23">
         <f>SUM(G4:G11)</f>
@@ -1090,7 +1087,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="26"/>
       <c r="D13" s="26"/>
@@ -1112,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>4</v>
@@ -1135,10 +1132,10 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2">
@@ -1150,12 +1147,12 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1211,11 +1208,11 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -1230,11 +1227,11 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -1247,7 +1244,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1263,10 +1260,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="9">
         <v>2</v>
@@ -1279,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1288,7 +1285,7 @@
       <c r="D25" s="20"/>
       <c r="E25" s="21"/>
       <c r="F25" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="23">
         <f>SUM(G15:G24)</f>
@@ -1319,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>4</v>
@@ -1329,32 +1326,32 @@
       <c r="B28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>69</v>
+      <c r="C28" t="s">
+        <v>68</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" s="13">
         <v>1</v>
       </c>
       <c r="F28" s="14">
-        <v>6.36</v>
+        <v>12.62</v>
       </c>
       <c r="G28" s="14">
         <f t="shared" ref="G28:G36" si="2">F28*E28</f>
-        <v>6.36</v>
+        <v>12.62</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13">
         <v>5</v>
@@ -1365,18 +1362,18 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E30" s="2">
         <v>8</v>
@@ -1387,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
@@ -1395,73 +1392,65 @@
         <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" s="7">
-        <v>17.95</v>
+        <v>49.95</v>
       </c>
       <c r="G31" s="7">
         <f t="shared" si="2"/>
-        <v>17.95</v>
+        <v>49.95</v>
+      </c>
+      <c r="H31" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
       </c>
       <c r="F32" s="7">
-        <v>49.95</v>
+        <v>33</v>
       </c>
       <c r="G32" s="7">
         <f t="shared" si="2"/>
-        <v>49.95</v>
-      </c>
-      <c r="H32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="7">
-        <v>33</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7">
@@ -1469,125 +1458,133 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="7"/>
+      <c r="C35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.35</v>
+      </c>
       <c r="G35" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="9">
         <v>1</v>
       </c>
       <c r="F36" s="7">
-        <v>1.51</v>
+        <v>0.63</v>
       </c>
       <c r="G36" s="7">
         <f t="shared" si="2"/>
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="9" t="s">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="23">
+        <f>SUM(G28:G36)</f>
+        <v>96.549999999999983</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="27"/>
+    </row>
+    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="9">
+      <c r="D40" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="13">
         <v>1</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" s="23">
-        <f>SUM(G28:G37)</f>
-        <v>109.05000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-    </row>
-    <row r="40" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="16" t="s">
+      <c r="F40" s="14">
+        <v>150</v>
+      </c>
+      <c r="G40" s="14">
+        <f t="shared" ref="G40:G51" si="3">F40*E40</f>
+        <v>150</v>
+      </c>
+      <c r="H40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2">
         <v>1</v>
       </c>
-      <c r="F40" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="13" t="s">
+      <c r="F41" s="7"/>
+      <c r="G41" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E41" s="13">
-        <v>1</v>
-      </c>
-      <c r="F41" s="14">
-        <v>150</v>
-      </c>
-      <c r="G41" s="14">
-        <f t="shared" ref="G41:G52" si="3">F41*E41</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1600,14 +1597,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="s">
-        <v>25</v>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7">
@@ -1615,14 +1612,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7">
@@ -1630,9 +1627,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" s="2" t="s">
-        <v>28</v>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -1645,24 +1642,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="2">
-        <v>1</v>
-      </c>
+      <c r="E46" s="2"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1673,9 +1668,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1688,11 +1683,13 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7">
         <f t="shared" si="3"/>
@@ -1701,12 +1698,12 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" s="4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7">
@@ -1716,13 +1713,11 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="2">
-        <v>4</v>
-      </c>
+      <c r="E51" s="2"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7">
         <f t="shared" si="3"/>
@@ -1730,28 +1725,15 @@
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="7"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="G52" s="7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="10"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G53" s="7">
-        <f>SUM(G41:G52)</f>
+        <f>SUM(G40:G51)</f>
         <v>150</v>
       </c>
     </row>
@@ -1760,7 +1742,7 @@
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B38:G38"/>
     <mergeCell ref="L7:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Spice and Updated budget
</commit_message>
<xml_diff>
--- a/CHIPS Documents/CHIPS Budget.xlsx
+++ b/CHIPS Documents/CHIPS Budget.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
   <si>
     <t>Item</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Section Total:</t>
   </si>
   <si>
-    <t>Coax Connector</t>
-  </si>
-  <si>
     <t>Programming Header</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>497-6003-6-ND</t>
+  </si>
+  <si>
+    <t>BNC</t>
   </si>
 </sst>
 </file>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -940,7 +940,7 @@
       </c>
       <c r="K4" s="5">
         <f>SUM(G4:G11,G15:G22,G26:G33,G37:G49)</f>
-        <v>1947.6119999999999</v>
+        <v>1963.0359999999998</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
@@ -1144,29 +1144,31 @@
         <v>13</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="13">
-        <v>32</v>
-      </c>
-      <c r="F15" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.96399999999999997</v>
+      </c>
       <c r="G15" s="14">
         <f t="shared" ref="G15:G22" si="1">F15*E15</f>
-        <v>0</v>
+        <v>15.423999999999999</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -1177,15 +1179,15 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>35</v>
@@ -1201,7 +1203,7 @@
         <v>95.311999999999998</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.35">
@@ -1273,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>34</v>
@@ -1289,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1302,7 +1304,7 @@
       </c>
       <c r="G23" s="23">
         <f>SUM(G15:G22)</f>
-        <v>161.31200000000001</v>
+        <v>176.73599999999999</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
@@ -1340,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>35</v>
@@ -1355,16 +1357,19 @@
         <f t="shared" ref="G26:G33" si="2">F26*E26</f>
         <v>12.62</v>
       </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="13">
         <v>5</v>
@@ -1375,18 +1380,18 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E28" s="2">
         <v>8</v>
@@ -1397,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
@@ -1405,10 +1410,10 @@
         <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -1421,7 +1426,7 @@
         <v>49.95</v>
       </c>
       <c r="H29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.35">
@@ -1463,7 +1468,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>35</v>
@@ -1481,10 +1486,10 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>35</v>
@@ -1515,7 +1520,7 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -1564,7 +1569,7 @@
         <v>150</v>
       </c>
       <c r="H37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.35">
@@ -1572,7 +1577,7 @@
         <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>35</v>
@@ -1593,7 +1598,7 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>35</v>
@@ -1611,10 +1616,10 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" t="s">
-        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>35</v>
@@ -1632,10 +1637,10 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>35</v>
@@ -1656,7 +1661,7 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>35</v>
@@ -1674,10 +1679,10 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>35</v>

</xml_diff>